<commit_message>
Final commit ,sprint 3 ending + project ending
</commit_message>
<xml_diff>
--- a/Documentation/Documentation finale/Document de base/Journal de travail Renaud Grégory TPI.xlsx
+++ b/Documentation/Documentation finale/Document de base/Journal de travail Renaud Grégory TPI.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduvaud-my.sharepoint.com/personal/ph62ldr_eduvaud_ch/Documents/TPI/Semaine 3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduvaud-my.sharepoint.com/personal/ph62ldr_eduvaud_ch/Documents/TPI/Documentation finale/Document de base/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="215" documentId="13_ncr:1_{E93AF827-F335-4273-9BF2-1B7E35411D1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57B80893-E69B-4765-AAC2-36381B3B9A44}"/>
+  <xr:revisionPtr revIDLastSave="253" documentId="13_ncr:1_{E93AF827-F335-4273-9BF2-1B7E35411D1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC3C08DF-4846-4B29-8F8F-2DF12E374780}"/>
   <bookViews>
     <workbookView xWindow="1515" yWindow="-15870" windowWidth="25440" windowHeight="15390" xr2:uid="{E616EBF9-A1E1-4B05-B307-B39FC77B0801}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="217">
   <si>
     <t>Date</t>
   </si>
@@ -674,6 +674,24 @@
   </si>
   <si>
     <t>Rédaction du manuel d'utilisation</t>
+  </si>
+  <si>
+    <t>Vérification des fichiers finaux</t>
+  </si>
+  <si>
+    <t>Vérification du script SQL de création de la DB</t>
+  </si>
+  <si>
+    <t>Vérification du rapport basé sur la grille d'évaluation</t>
+  </si>
+  <si>
+    <t>Dernier test de l'application</t>
+  </si>
+  <si>
+    <t>Impression des documents et reliure</t>
+  </si>
+  <si>
+    <t>Préparation pour l'envoi final papier et dernier push Github</t>
   </si>
 </sst>
 </file>
@@ -1342,13 +1360,13 @@
                   <c:v>1.7187500000000009</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.70833333333333326</c:v>
+                  <c:v>0.9409722222222221</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.10069444444444448</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.15972222222222221</c:v>
+                  <c:v>0.1875</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.31944444444444442</c:v>
@@ -2046,10 +2064,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{276EA92B-46E1-49DE-A871-36F19432AE6D}" name="Catégorie" displayName="Catégorie" ref="A1:A42" totalsRowShown="0" dataDxfId="4">
   <autoFilter ref="A1:A42" xr:uid="{276EA92B-46E1-49DE-A871-36F19432AE6D}"/>
@@ -2363,8 +2377,8 @@
   <dimension ref="A1:I1196"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A128" sqref="A128"/>
+      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A135" sqref="A135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5581,99 +5595,171 @@
       <c r="I127" s="14"/>
     </row>
     <row r="128" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="5"/>
-      <c r="B128" s="5"/>
-      <c r="C128" s="5"/>
+      <c r="A128" s="3">
+        <v>45790</v>
+      </c>
+      <c r="B128" s="4">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="C128" s="4">
+        <v>0.40277777777777779</v>
+      </c>
       <c r="D128" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E128" s="5"/>
-      <c r="F128" s="9"/>
-      <c r="G128" s="9"/>
+        <v>1.3888888888888895E-2</v>
+      </c>
+      <c r="E128" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F128" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="G128" s="9" t="s">
+        <v>212</v>
+      </c>
       <c r="H128" s="9"/>
       <c r="I128" s="14"/>
     </row>
     <row r="129" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="5"/>
-      <c r="B129" s="5"/>
-      <c r="C129" s="5"/>
+      <c r="A129" s="3">
+        <v>45790</v>
+      </c>
+      <c r="B129" s="4">
+        <v>0.4201388888888889</v>
+      </c>
+      <c r="C129" s="4">
+        <v>0.44444444444444442</v>
+      </c>
       <c r="D129" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E129" s="5"/>
-      <c r="F129" s="9"/>
+        <v>2.4305555555555525E-2</v>
+      </c>
+      <c r="E129" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F129" s="9" t="s">
+        <v>174</v>
+      </c>
       <c r="G129" s="9"/>
       <c r="H129" s="9"/>
       <c r="I129" s="14"/>
     </row>
     <row r="130" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="5"/>
-      <c r="B130" s="5"/>
-      <c r="C130" s="5"/>
+      <c r="A130" s="3">
+        <v>45790</v>
+      </c>
+      <c r="B130" s="4">
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="C130" s="4">
+        <v>0.62152777777777779</v>
+      </c>
       <c r="D130" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E130" s="5"/>
-      <c r="F130" s="9"/>
+        <v>6.597222222222221E-2</v>
+      </c>
+      <c r="E130" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F130" s="9" t="s">
+        <v>213</v>
+      </c>
       <c r="G130" s="9"/>
       <c r="H130" s="9"/>
       <c r="I130" s="14"/>
     </row>
     <row r="131" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="5"/>
-      <c r="B131" s="5"/>
-      <c r="C131" s="5"/>
+      <c r="A131" s="3">
+        <v>45790</v>
+      </c>
+      <c r="B131" s="4">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="C131" s="4">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="D131" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E131" s="5"/>
-      <c r="F131" s="9"/>
+        <v>3.819444444444442E-2</v>
+      </c>
+      <c r="E131" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F131" s="9" t="s">
+        <v>213</v>
+      </c>
       <c r="G131" s="9"/>
       <c r="H131" s="9"/>
       <c r="I131" s="14"/>
     </row>
     <row r="132" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="5"/>
-      <c r="B132" s="5"/>
-      <c r="C132" s="5"/>
+      <c r="A132" s="3">
+        <v>45790</v>
+      </c>
+      <c r="B132" s="4">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C132" s="4">
+        <v>0.69444444444444442</v>
+      </c>
       <c r="D132" s="4">
         <f t="shared" ref="D132:D166" si="5">C132-B132</f>
-        <v>0</v>
-      </c>
-      <c r="E132" s="5"/>
-      <c r="F132" s="9"/>
+        <v>2.777777777777779E-2</v>
+      </c>
+      <c r="E132" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F132" s="9" t="s">
+        <v>214</v>
+      </c>
       <c r="G132" s="9"/>
       <c r="H132" s="9"/>
       <c r="I132" s="14"/>
     </row>
     <row r="133" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="5"/>
-      <c r="B133" s="5"/>
-      <c r="C133" s="5"/>
+      <c r="A133" s="3">
+        <v>45791</v>
+      </c>
+      <c r="B133" s="4">
+        <v>0.34375</v>
+      </c>
+      <c r="C133" s="4">
+        <v>0.40972222222222221</v>
+      </c>
       <c r="D133" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E133" s="5"/>
-      <c r="F133" s="9"/>
+        <v>6.597222222222221E-2</v>
+      </c>
+      <c r="E133" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F133" s="9" t="s">
+        <v>215</v>
+      </c>
       <c r="G133" s="9"/>
       <c r="H133" s="9"/>
       <c r="I133" s="14"/>
     </row>
-    <row r="134" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="5"/>
-      <c r="B134" s="5"/>
-      <c r="C134" s="5"/>
+    <row r="134" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A134" s="3">
+        <v>45791</v>
+      </c>
+      <c r="B134" s="4">
+        <v>0.4201388888888889</v>
+      </c>
+      <c r="C134" s="4">
+        <v>0.44444444444444442</v>
+      </c>
       <c r="D134" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E134" s="5"/>
-      <c r="F134" s="9"/>
+        <v>2.4305555555555525E-2</v>
+      </c>
+      <c r="E134" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F134" s="9" t="s">
+        <v>216</v>
+      </c>
       <c r="G134" s="9"/>
       <c r="H134" s="9"/>
       <c r="I134" s="14"/>
@@ -18185,7 +18271,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E7"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18209,7 +18295,7 @@
       </c>
       <c r="E1" s="17">
         <f>SUM(B2:B7)</f>
-        <v>3.3715277777777786</v>
+        <v>3.6319444444444455</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -18223,7 +18309,7 @@
       </c>
       <c r="E2" s="18">
         <f>SUM(B2:B7)</f>
-        <v>3.3715277777777786</v>
+        <v>3.6319444444444455</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -18233,7 +18319,7 @@
       </c>
       <c r="B3" s="11">
         <f>SUMIF(Journal!E2:E980, Résumé!A3,Journal!D2:D980)</f>
-        <v>0.70833333333333326</v>
+        <v>0.9409722222222221</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -18253,7 +18339,7 @@
       </c>
       <c r="B5" s="11">
         <f>SUMIF(Journal!E2:E982, Résumé!A5,Journal!D2:D982)</f>
-        <v>0.15972222222222221</v>
+        <v>0.1875</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>